<commit_message>
update employee and login
</commit_message>
<xml_diff>
--- a/Database ToCoShopvs.xlsx
+++ b/Database ToCoShopvs.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10512"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
     <sheet name="Orders" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="145">
   <si>
     <t>No.</t>
   </si>
@@ -435,12 +435,27 @@
   </si>
   <si>
     <t>number</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
+  </si>
+  <si>
+    <t>NAM/NU/KHONG_XAC_DINH</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>KHONG_XAC_DINH</t>
+  </si>
+  <si>
+    <t>Not allow update -UNIQUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -559,7 +574,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,12 +638,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
@@ -829,7 +838,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1018,16 +1027,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1046,6 +1045,79 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1053,85 +1125,13 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1440,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:XFD127"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="H90" sqref="H90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1452,35 +1452,35 @@
     <col min="4" max="4" width="19.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23" style="1" customWidth="1"/>
     <col min="8" max="8" width="48.44140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="110"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111"/>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
-      <c r="G3" s="111"/>
-      <c r="H3" s="111"/>
-      <c r="I3" s="111"/>
+      <c r="A3" s="113"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
     </row>
     <row r="4" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -1621,28 +1621,28 @@
       <c r="I9" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="104"/>
-      <c r="C12" s="104"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
+      <c r="B12" s="114"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="114"/>
+      <c r="E12" s="114"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="114"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="105"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
+      <c r="A13" s="115"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="39" t="s">
@@ -1819,28 +1819,28 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="112" t="s">
+      <c r="A24" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="112"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="112"/>
-      <c r="I24" s="112"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="116"/>
     </row>
     <row r="25" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="112"/>
-      <c r="B25" s="112"/>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="112"/>
-      <c r="H25" s="112"/>
-      <c r="I25" s="112"/>
+      <c r="A25" s="116"/>
+      <c r="B25" s="116"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
+      <c r="E25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="116"/>
+      <c r="H25" s="116"/>
+      <c r="I25" s="116"/>
     </row>
     <row r="26" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -2003,7 +2003,7 @@
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="101">
+      <c r="A33" s="120">
         <v>7</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -2020,7 +2020,7 @@
       <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="102"/>
+      <c r="A34" s="121"/>
       <c r="B34" s="4" t="s">
         <v>26</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="102"/>
+      <c r="A35" s="121"/>
       <c r="B35" s="4" t="s">
         <v>25</v>
       </c>
@@ -2060,7 +2060,7 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="102"/>
+      <c r="A36" s="121"/>
       <c r="B36" s="4" t="s">
         <v>54</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="102"/>
+      <c r="A37" s="121"/>
       <c r="B37" s="4" t="s">
         <v>53</v>
       </c>
@@ -2098,7 +2098,7 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A38" s="102"/>
+      <c r="A38" s="121"/>
       <c r="B38" s="23" t="s">
         <v>27</v>
       </c>
@@ -2106,16 +2106,16 @@
         <v>61</v>
       </c>
       <c r="D38" s="25"/>
-      <c r="E38" s="94" t="s">
+      <c r="E38" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="95"/>
-      <c r="G38" s="95"/>
-      <c r="H38" s="95"/>
-      <c r="I38" s="96"/>
+      <c r="F38" s="91"/>
+      <c r="G38" s="91"/>
+      <c r="H38" s="91"/>
+      <c r="I38" s="92"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="102"/>
+      <c r="A39" s="121"/>
       <c r="B39" s="26" t="s">
         <v>51</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="102"/>
+      <c r="A40" s="121"/>
       <c r="B40" s="26" t="s">
         <v>119</v>
       </c>
@@ -2153,7 +2153,7 @@
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="102"/>
+      <c r="A41" s="121"/>
       <c r="B41" s="26" t="s">
         <v>120</v>
       </c>
@@ -2172,7 +2172,7 @@
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="103"/>
+      <c r="A42" s="122"/>
       <c r="B42" s="26" t="s">
         <v>52</v>
       </c>
@@ -2191,7 +2191,7 @@
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="101">
+      <c r="A43" s="120">
         <v>8</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -2210,7 +2210,7 @@
       <c r="I43" s="8"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="102"/>
+      <c r="A44" s="121"/>
       <c r="B44" s="4" t="s">
         <v>100</v>
       </c>
@@ -2229,7 +2229,7 @@
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="102"/>
+      <c r="A45" s="121"/>
       <c r="B45" s="4" t="s">
         <v>54</v>
       </c>
@@ -2248,7 +2248,7 @@
       <c r="I45" s="4"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="102"/>
+      <c r="A46" s="121"/>
       <c r="B46" s="4" t="s">
         <v>53</v>
       </c>
@@ -2267,7 +2267,7 @@
       <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="102"/>
+      <c r="A47" s="121"/>
       <c r="B47" s="4" t="s">
         <v>26</v>
       </c>
@@ -2286,7 +2286,7 @@
       <c r="I47" s="4"/>
     </row>
     <row r="48" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A48" s="102"/>
+      <c r="A48" s="121"/>
       <c r="B48" s="23" t="s">
         <v>27</v>
       </c>
@@ -2294,18 +2294,18 @@
         <v>61</v>
       </c>
       <c r="D48" s="25"/>
-      <c r="E48" s="94" t="s">
+      <c r="E48" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="F48" s="107" t="s">
+      <c r="F48" s="118" t="s">
         <v>74</v>
       </c>
-      <c r="G48" s="107"/>
-      <c r="H48" s="107"/>
-      <c r="I48" s="108"/>
+      <c r="G48" s="118"/>
+      <c r="H48" s="118"/>
+      <c r="I48" s="119"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="102"/>
+      <c r="A49" s="121"/>
       <c r="B49" s="26" t="s">
         <v>51</v>
       </c>
@@ -2324,7 +2324,7 @@
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="102"/>
+      <c r="A50" s="121"/>
       <c r="B50" s="26" t="s">
         <v>119</v>
       </c>
@@ -2343,7 +2343,7 @@
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="102"/>
+      <c r="A51" s="121"/>
       <c r="B51" s="26" t="s">
         <v>120</v>
       </c>
@@ -2362,7 +2362,7 @@
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="102"/>
+      <c r="A52" s="121"/>
       <c r="B52" s="26" t="s">
         <v>52</v>
       </c>
@@ -2381,7 +2381,7 @@
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="103"/>
+      <c r="A53" s="122"/>
       <c r="B53" s="4" t="s">
         <v>49</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="101">
+      <c r="A54" s="120">
         <v>9</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -2419,7 +2419,7 @@
       <c r="I54" s="8"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="102"/>
+      <c r="A55" s="121"/>
       <c r="B55" s="4" t="s">
         <v>55</v>
       </c>
@@ -2436,7 +2436,7 @@
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="1:9" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A56" s="102"/>
+      <c r="A56" s="121"/>
       <c r="B56" s="23" t="s">
         <v>57</v>
       </c>
@@ -2444,16 +2444,16 @@
         <v>38</v>
       </c>
       <c r="D56" s="25"/>
-      <c r="E56" s="106" t="s">
+      <c r="E56" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="107"/>
-      <c r="G56" s="107"/>
-      <c r="H56" s="107"/>
-      <c r="I56" s="108"/>
+      <c r="F56" s="118"/>
+      <c r="G56" s="118"/>
+      <c r="H56" s="118"/>
+      <c r="I56" s="119"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="102"/>
+      <c r="A57" s="121"/>
       <c r="B57" s="26" t="s">
         <v>58</v>
       </c>
@@ -2470,7 +2470,7 @@
       <c r="I57" s="4"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="102"/>
+      <c r="A58" s="121"/>
       <c r="B58" s="26" t="s">
         <v>95</v>
       </c>
@@ -2487,7 +2487,7 @@
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="102"/>
+      <c r="A59" s="121"/>
       <c r="B59" s="26" t="s">
         <v>59</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="103"/>
+      <c r="A60" s="122"/>
       <c r="B60" s="26" t="s">
         <v>60</v>
       </c>
@@ -2519,13 +2519,13 @@
       <c r="E60" s="7"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
-      <c r="H60" s="91" t="s">
+      <c r="H60" s="87" t="s">
         <v>98</v>
       </c>
       <c r="I60" s="4"/>
     </row>
     <row r="61" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="109">
+      <c r="A61" s="127">
         <v>10</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -2542,7 +2542,7 @@
       <c r="I61" s="8"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="109"/>
+      <c r="A62" s="127"/>
       <c r="B62" s="4" t="s">
         <v>122</v>
       </c>
@@ -2561,7 +2561,7 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="109"/>
+      <c r="A63" s="127"/>
       <c r="B63" s="4" t="s">
         <v>127</v>
       </c>
@@ -2576,7 +2576,7 @@
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="109"/>
+      <c r="A64" s="127"/>
       <c r="B64" s="4" t="s">
         <v>41</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="109"/>
+      <c r="A65" s="127"/>
       <c r="B65" s="4" t="s">
         <v>43</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="109"/>
+      <c r="A66" s="127"/>
       <c r="B66" s="4" t="s">
         <v>44</v>
       </c>
@@ -2621,7 +2621,7 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="101">
+      <c r="A67" s="120">
         <v>11</v>
       </c>
       <c r="B67" s="8" t="s">
@@ -2638,7 +2638,7 @@
       <c r="I67" s="8"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="102"/>
+      <c r="A68" s="121"/>
       <c r="B68" s="4" t="s">
         <v>105</v>
       </c>
@@ -2657,7 +2657,7 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="102"/>
+      <c r="A69" s="121"/>
       <c r="B69" s="4" t="s">
         <v>106</v>
       </c>
@@ -2676,7 +2676,7 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="103"/>
+      <c r="A70" s="122"/>
       <c r="B70" s="4" t="s">
         <v>97</v>
       </c>
@@ -2693,28 +2693,28 @@
       <c r="I70" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="104" t="s">
+      <c r="A73" s="114" t="s">
         <v>62</v>
       </c>
-      <c r="B73" s="104"/>
-      <c r="C73" s="104"/>
-      <c r="D73" s="104"/>
-      <c r="E73" s="104"/>
-      <c r="F73" s="104"/>
-      <c r="G73" s="104"/>
-      <c r="H73" s="104"/>
-      <c r="I73" s="104"/>
+      <c r="B73" s="114"/>
+      <c r="C73" s="114"/>
+      <c r="D73" s="114"/>
+      <c r="E73" s="114"/>
+      <c r="F73" s="114"/>
+      <c r="G73" s="114"/>
+      <c r="H73" s="114"/>
+      <c r="I73" s="114"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="105"/>
-      <c r="B74" s="105"/>
-      <c r="C74" s="105"/>
-      <c r="D74" s="105"/>
-      <c r="E74" s="105"/>
-      <c r="F74" s="105"/>
-      <c r="G74" s="105"/>
-      <c r="H74" s="105"/>
-      <c r="I74" s="105"/>
+      <c r="A74" s="115"/>
+      <c r="B74" s="115"/>
+      <c r="C74" s="115"/>
+      <c r="D74" s="115"/>
+      <c r="E74" s="115"/>
+      <c r="F74" s="115"/>
+      <c r="G74" s="115"/>
+      <c r="H74" s="115"/>
+      <c r="I74" s="115"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="39" t="s">
@@ -2807,7 +2807,7 @@
       <c r="I78" s="49"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="92">
+      <c r="A79" s="88">
         <f t="shared" ref="A79:A82" si="3">A78+1</f>
         <v>4</v>
       </c>
@@ -2831,7 +2831,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B80" s="93" t="s">
+      <c r="B80" s="89" t="s">
         <v>103</v>
       </c>
       <c r="C80" s="46" t="s">
@@ -2889,28 +2889,28 @@
       <c r="I82" s="44"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="110" t="s">
+      <c r="A86" s="112" t="s">
         <v>65</v>
       </c>
-      <c r="B86" s="110"/>
-      <c r="C86" s="110"/>
-      <c r="D86" s="110"/>
-      <c r="E86" s="110"/>
-      <c r="F86" s="110"/>
-      <c r="G86" s="110"/>
-      <c r="H86" s="110"/>
-      <c r="I86" s="110"/>
+      <c r="B86" s="112"/>
+      <c r="C86" s="112"/>
+      <c r="D86" s="112"/>
+      <c r="E86" s="112"/>
+      <c r="F86" s="112"/>
+      <c r="G86" s="112"/>
+      <c r="H86" s="112"/>
+      <c r="I86" s="112"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="113"/>
-      <c r="B87" s="113"/>
-      <c r="C87" s="113"/>
-      <c r="D87" s="113"/>
-      <c r="E87" s="113"/>
-      <c r="F87" s="113"/>
-      <c r="G87" s="113"/>
-      <c r="H87" s="113"/>
-      <c r="I87" s="113"/>
+      <c r="A87" s="117"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="117"/>
+      <c r="D87" s="117"/>
+      <c r="E87" s="117"/>
+      <c r="F87" s="117"/>
+      <c r="G87" s="117"/>
+      <c r="H87" s="117"/>
+      <c r="I87" s="117"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="33" t="s">
@@ -2979,6 +2979,9 @@
       <c r="E90" s="32"/>
       <c r="F90" s="30"/>
       <c r="G90" s="30"/>
+      <c r="H90" s="128" t="s">
+        <v>144</v>
+      </c>
       <c r="I90" s="30"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
@@ -3051,28 +3054,28 @@
       <c r="A95" s="61"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="110" t="s">
+      <c r="A99" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="B99" s="110"/>
-      <c r="C99" s="110"/>
-      <c r="D99" s="110"/>
-      <c r="E99" s="110"/>
-      <c r="F99" s="110"/>
-      <c r="G99" s="110"/>
-      <c r="H99" s="110"/>
-      <c r="I99" s="110"/>
+      <c r="B99" s="112"/>
+      <c r="C99" s="112"/>
+      <c r="D99" s="112"/>
+      <c r="E99" s="112"/>
+      <c r="F99" s="112"/>
+      <c r="G99" s="112"/>
+      <c r="H99" s="112"/>
+      <c r="I99" s="112"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="113"/>
-      <c r="B100" s="113"/>
-      <c r="C100" s="113"/>
-      <c r="D100" s="113"/>
-      <c r="E100" s="113"/>
-      <c r="F100" s="113"/>
-      <c r="G100" s="113"/>
-      <c r="H100" s="113"/>
-      <c r="I100" s="113"/>
+      <c r="A100" s="117"/>
+      <c r="B100" s="117"/>
+      <c r="C100" s="117"/>
+      <c r="D100" s="117"/>
+      <c r="E100" s="117"/>
+      <c r="F100" s="117"/>
+      <c r="G100" s="117"/>
+      <c r="H100" s="117"/>
+      <c r="I100" s="117"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="33" t="s">
@@ -3228,13 +3231,13 @@
       <c r="I107" s="68"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="98" t="s">
+      <c r="A111" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="B111" s="99"/>
-      <c r="C111" s="99"/>
-      <c r="D111" s="99"/>
-      <c r="E111" s="99"/>
+      <c r="B111" s="124"/>
+      <c r="C111" s="124"/>
+      <c r="D111" s="124"/>
+      <c r="E111" s="124"/>
       <c r="F111" s="71"/>
       <c r="G111" s="71"/>
       <c r="H111" s="71"/>
@@ -3305,7 +3308,9 @@
       </c>
       <c r="E114" s="80"/>
       <c r="F114" s="77"/>
-      <c r="G114" s="77"/>
+      <c r="G114" s="77" t="s">
+        <v>121</v>
+      </c>
       <c r="H114" s="77"/>
       <c r="I114" s="77"/>
     </row>
@@ -3324,7 +3329,9 @@
       </c>
       <c r="E115" s="80"/>
       <c r="F115" s="77"/>
-      <c r="G115" s="77"/>
+      <c r="G115" s="77" t="s">
+        <v>121</v>
+      </c>
       <c r="H115" s="77"/>
       <c r="I115" s="77"/>
     </row>
@@ -3364,7 +3371,9 @@
       </c>
       <c r="E117" s="80"/>
       <c r="F117" s="77"/>
-      <c r="G117" s="77"/>
+      <c r="G117" s="77" t="s">
+        <v>121</v>
+      </c>
       <c r="H117" s="62" t="s">
         <v>68</v>
       </c>
@@ -3392,395 +3401,415 @@
       <c r="I118" s="77"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="86">
+      <c r="A119" s="82">
         <v>7</v>
       </c>
-      <c r="B119" s="86" t="s">
+      <c r="B119" s="82" t="s">
         <v>82</v>
       </c>
-      <c r="C119" s="87" t="s">
+      <c r="C119" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="D119" s="88"/>
-      <c r="E119" s="89" t="s">
+      <c r="D119" s="84"/>
+      <c r="E119" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="F119" s="86"/>
-      <c r="G119" s="86"/>
-      <c r="H119" s="86"/>
-      <c r="I119" s="86"/>
+      <c r="F119" s="82"/>
+      <c r="G119" s="82"/>
+      <c r="H119" s="82"/>
+      <c r="I119" s="82"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="82"/>
-      <c r="B120" s="82"/>
-      <c r="C120" s="83"/>
+      <c r="A120" s="82">
+        <v>8</v>
+      </c>
+      <c r="B120" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="C120" s="83" t="s">
+        <v>14</v>
+      </c>
       <c r="D120" s="84"/>
-      <c r="E120" s="85"/>
+      <c r="E120" s="85" t="s">
+        <v>17</v>
+      </c>
       <c r="F120" s="82"/>
       <c r="G120" s="82"/>
       <c r="H120" s="82"/>
       <c r="I120" s="82"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="82"/>
-      <c r="B121" s="82"/>
-      <c r="C121" s="83"/>
+      <c r="A121" s="82">
+        <v>9</v>
+      </c>
+      <c r="B121" s="82" t="s">
+        <v>142</v>
+      </c>
+      <c r="C121" s="83" t="s">
+        <v>14</v>
+      </c>
       <c r="D121" s="84"/>
-      <c r="E121" s="85"/>
+      <c r="E121" s="85" t="s">
+        <v>17</v>
+      </c>
       <c r="F121" s="82"/>
-      <c r="G121" s="82"/>
-      <c r="H121" s="82"/>
+      <c r="G121" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="H121" s="82" t="s">
+        <v>141</v>
+      </c>
       <c r="I121" s="82"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="90"/>
-      <c r="B122" s="90"/>
-      <c r="C122" s="90"/>
-      <c r="D122" s="90"/>
-      <c r="E122" s="90"/>
-      <c r="F122" s="90"/>
-      <c r="G122" s="90"/>
-      <c r="H122" s="90"/>
-      <c r="I122" s="90"/>
+      <c r="A122" s="86"/>
+      <c r="B122" s="86"/>
+      <c r="C122" s="86"/>
+      <c r="D122" s="86"/>
+      <c r="E122" s="86"/>
+      <c r="F122" s="86"/>
+      <c r="G122" s="86"/>
+      <c r="H122" s="86"/>
+      <c r="I122" s="86"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="100" t="s">
+      <c r="A123" s="125" t="s">
         <v>83</v>
       </c>
-      <c r="B123" s="99"/>
-      <c r="C123" s="99"/>
-      <c r="D123" s="99"/>
-      <c r="E123" s="99"/>
+      <c r="B123" s="124"/>
+      <c r="C123" s="124"/>
+      <c r="D123" s="124"/>
+      <c r="E123" s="124"/>
       <c r="F123" s="81"/>
       <c r="G123" s="81"/>
       <c r="H123" s="81"/>
       <c r="I123" s="81"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="116" t="s">
+      <c r="A124" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B124" s="116" t="s">
+      <c r="B124" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="C124" s="116" t="s">
+      <c r="C124" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="D124" s="116" t="s">
+      <c r="D124" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="E124" s="116" t="s">
+      <c r="E124" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="F124" s="116" t="s">
+      <c r="F124" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="G124" s="116" t="s">
+      <c r="G124" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="H124" s="116" t="s">
+      <c r="H124" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="I124" s="116" t="s">
+      <c r="I124" s="96" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="117">
+      <c r="A125" s="97">
         <v>1</v>
       </c>
-      <c r="B125" s="117" t="s">
+      <c r="B125" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="C125" s="116" t="s">
+      <c r="C125" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="D125" s="118"/>
-      <c r="E125" s="119"/>
-      <c r="F125" s="117" t="s">
+      <c r="D125" s="98"/>
+      <c r="E125" s="99"/>
+      <c r="F125" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="G125" s="117"/>
-      <c r="H125" s="117" t="s">
+      <c r="G125" s="97"/>
+      <c r="H125" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="I125" s="117"/>
+      <c r="I125" s="97"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="117">
+      <c r="A126" s="97">
         <v>2</v>
       </c>
-      <c r="B126" s="117" t="s">
+      <c r="B126" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="C126" s="116" t="s">
-        <v>14</v>
-      </c>
-      <c r="D126" s="118">
+      <c r="C126" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="98">
         <v>50</v>
       </c>
-      <c r="E126" s="119"/>
-      <c r="F126" s="117"/>
-      <c r="G126" s="117"/>
-      <c r="H126" s="117"/>
-      <c r="I126" s="117"/>
-    </row>
-    <row r="127" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="125">
+      <c r="E126" s="99"/>
+      <c r="F126" s="97"/>
+      <c r="G126" s="97"/>
+      <c r="H126" s="97"/>
+      <c r="I126" s="97"/>
+    </row>
+    <row r="127" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="105">
         <v>3</v>
       </c>
-      <c r="B127" s="125" t="s">
+      <c r="B127" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="C127" s="126" t="s">
+      <c r="C127" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="D127" s="127"/>
-      <c r="E127" s="128"/>
-      <c r="F127" s="125"/>
-      <c r="G127" s="125">
+      <c r="D127" s="107"/>
+      <c r="E127" s="108"/>
+      <c r="F127" s="105"/>
+      <c r="G127" s="105">
         <v>0</v>
       </c>
-      <c r="H127" s="125" t="s">
+      <c r="H127" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="I127" s="125"/>
-    </row>
-    <row r="128" spans="1:9" s="124" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="120">
+      <c r="I127" s="105"/>
+    </row>
+    <row r="128" spans="1:9" s="104" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="100">
         <v>4</v>
       </c>
-      <c r="B128" s="120" t="s">
+      <c r="B128" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="C128" s="121" t="s">
+      <c r="C128" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="D128" s="122"/>
-      <c r="E128" s="123"/>
-      <c r="F128" s="120"/>
-      <c r="G128" s="120">
+      <c r="D128" s="102"/>
+      <c r="E128" s="103"/>
+      <c r="F128" s="100"/>
+      <c r="G128" s="100">
         <v>0</v>
       </c>
-      <c r="H128" s="120" t="s">
+      <c r="H128" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="I128" s="120"/>
-    </row>
-    <row r="129" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="125">
+      <c r="I128" s="100"/>
+    </row>
+    <row r="129" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="105">
         <v>5</v>
       </c>
-      <c r="B129" s="125" t="s">
+      <c r="B129" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="C129" s="126" t="s">
+      <c r="C129" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="D129" s="127"/>
-      <c r="E129" s="128"/>
-      <c r="F129" s="125"/>
-      <c r="G129" s="125">
+      <c r="D129" s="107"/>
+      <c r="E129" s="108"/>
+      <c r="F129" s="105"/>
+      <c r="G129" s="105">
         <v>0</v>
       </c>
-      <c r="H129" s="125"/>
-      <c r="I129" s="125"/>
+      <c r="H129" s="105"/>
+      <c r="I129" s="105"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" s="117">
+      <c r="A130" s="97">
         <v>6</v>
       </c>
-      <c r="B130" s="117" t="s">
+      <c r="B130" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="C130" s="116" t="s">
+      <c r="C130" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="D130" s="118"/>
-      <c r="E130" s="119"/>
-      <c r="F130" s="117" t="s">
+      <c r="D130" s="98"/>
+      <c r="E130" s="99"/>
+      <c r="F130" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="G130" s="117"/>
-      <c r="H130" s="117" t="s">
+      <c r="G130" s="97"/>
+      <c r="H130" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="I130" s="117"/>
+      <c r="I130" s="97"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A131" s="117">
+      <c r="A131" s="97">
         <v>7</v>
       </c>
-      <c r="B131" s="117" t="s">
+      <c r="B131" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="C131" s="116" t="s">
+      <c r="C131" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="D131" s="118"/>
-      <c r="E131" s="119"/>
-      <c r="F131" s="117" t="s">
+      <c r="D131" s="98"/>
+      <c r="E131" s="99"/>
+      <c r="F131" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="G131" s="117"/>
-      <c r="H131" s="117" t="s">
+      <c r="G131" s="97"/>
+      <c r="H131" s="97" t="s">
         <v>90</v>
       </c>
-      <c r="I131" s="117"/>
+      <c r="I131" s="97"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A132" s="117">
+      <c r="A132" s="97">
         <v>8</v>
       </c>
-      <c r="B132" s="117" t="s">
+      <c r="B132" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="C132" s="119" t="s">
-        <v>14</v>
-      </c>
-      <c r="D132" s="118" t="s">
+      <c r="C132" s="99" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="E132" s="119"/>
-      <c r="F132" s="117"/>
-      <c r="G132" s="117"/>
-      <c r="H132" s="117"/>
-      <c r="I132" s="117"/>
+      <c r="E132" s="99"/>
+      <c r="F132" s="97"/>
+      <c r="G132" s="97"/>
+      <c r="H132" s="97"/>
+      <c r="I132" s="97"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="117">
+      <c r="A133" s="97">
         <v>9</v>
       </c>
-      <c r="B133" s="117" t="s">
+      <c r="B133" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C133" s="116" t="s">
+      <c r="C133" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="D133" s="118"/>
-      <c r="E133" s="119"/>
-      <c r="F133" s="117"/>
-      <c r="G133" s="117"/>
-      <c r="H133" s="117"/>
-      <c r="I133" s="117" t="s">
+      <c r="D133" s="98"/>
+      <c r="E133" s="99"/>
+      <c r="F133" s="97"/>
+      <c r="G133" s="97"/>
+      <c r="H133" s="97"/>
+      <c r="I133" s="97" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" s="117">
+      <c r="A134" s="97">
         <v>10</v>
       </c>
-      <c r="B134" s="117" t="s">
+      <c r="B134" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="C134" s="116" t="s">
-        <v>14</v>
-      </c>
-      <c r="D134" s="118"/>
-      <c r="E134" s="119"/>
-      <c r="F134" s="117"/>
-      <c r="G134" s="117"/>
-      <c r="H134" s="117"/>
-      <c r="I134" s="117"/>
+      <c r="C134" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="98"/>
+      <c r="E134" s="99"/>
+      <c r="F134" s="97"/>
+      <c r="G134" s="97"/>
+      <c r="H134" s="97"/>
+      <c r="I134" s="97"/>
     </row>
     <row r="135" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="117">
+      <c r="A135" s="97">
         <v>11</v>
       </c>
-      <c r="B135" s="117" t="s">
+      <c r="B135" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="C135" s="119" t="s">
+      <c r="C135" s="99" t="s">
         <v>93</v>
       </c>
-      <c r="D135" s="118"/>
-      <c r="E135" s="119"/>
-      <c r="F135" s="117"/>
-      <c r="G135" s="117"/>
-      <c r="H135" s="117"/>
-      <c r="I135" s="117" t="s">
+      <c r="D135" s="98"/>
+      <c r="E135" s="99"/>
+      <c r="F135" s="97"/>
+      <c r="G135" s="97"/>
+      <c r="H135" s="97"/>
+      <c r="I135" s="97" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="136" spans="1:9" s="11" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="130">
+      <c r="A136" s="110">
         <v>12</v>
       </c>
-      <c r="B136" s="130" t="s">
+      <c r="B136" s="110" t="s">
         <v>137</v>
       </c>
-      <c r="C136" s="131" t="s">
+      <c r="C136" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="D136" s="130"/>
-      <c r="E136" s="130"/>
-      <c r="F136" s="130"/>
-      <c r="G136" s="130"/>
-      <c r="H136" s="130"/>
-      <c r="I136" s="130"/>
+      <c r="D136" s="110"/>
+      <c r="E136" s="110"/>
+      <c r="F136" s="110"/>
+      <c r="G136" s="110"/>
+      <c r="H136" s="110"/>
+      <c r="I136" s="110"/>
     </row>
     <row r="137" spans="1:9" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="114"/>
-      <c r="B137" s="114" t="s">
+      <c r="A137" s="94"/>
+      <c r="B137" s="94" t="s">
         <v>138</v>
       </c>
-      <c r="C137" s="115" t="s">
-        <v>14</v>
-      </c>
-      <c r="D137" s="114"/>
-      <c r="E137" s="114"/>
-      <c r="F137" s="114"/>
-      <c r="G137" s="114"/>
-      <c r="H137" s="114"/>
-      <c r="I137" s="114"/>
+      <c r="C137" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="94"/>
+      <c r="E137" s="94"/>
+      <c r="F137" s="94"/>
+      <c r="G137" s="94"/>
+      <c r="H137" s="94"/>
+      <c r="I137" s="94"/>
     </row>
     <row r="138" spans="1:9" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="114"/>
-      <c r="B138" s="114" t="s">
+      <c r="A138" s="94"/>
+      <c r="B138" s="94" t="s">
         <v>86</v>
       </c>
-      <c r="C138" s="115" t="s">
+      <c r="C138" s="95" t="s">
         <v>139</v>
       </c>
-      <c r="D138" s="114"/>
-      <c r="E138" s="114"/>
-      <c r="F138" s="114"/>
-      <c r="G138" s="114"/>
-      <c r="H138" s="114"/>
-      <c r="I138" s="114"/>
+      <c r="D138" s="94"/>
+      <c r="E138" s="94"/>
+      <c r="F138" s="94"/>
+      <c r="G138" s="94"/>
+      <c r="H138" s="94"/>
+      <c r="I138" s="94"/>
     </row>
     <row r="139" spans="1:9" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="114"/>
-      <c r="B139" s="114" t="s">
+      <c r="A139" s="94"/>
+      <c r="B139" s="94" t="s">
         <v>101</v>
       </c>
-      <c r="C139" s="115" t="s">
+      <c r="C139" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="D139" s="114"/>
-      <c r="E139" s="114"/>
-      <c r="F139" s="114"/>
-      <c r="G139" s="114"/>
-      <c r="H139" s="114"/>
-      <c r="I139" s="114"/>
+      <c r="D139" s="94"/>
+      <c r="E139" s="94"/>
+      <c r="F139" s="94"/>
+      <c r="G139" s="94"/>
+      <c r="H139" s="94"/>
+      <c r="I139" s="94"/>
     </row>
     <row r="140" spans="1:9" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="114"/>
-      <c r="B140" s="114" t="s">
+      <c r="A140" s="94"/>
+      <c r="B140" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="C140" s="114" t="s">
+      <c r="C140" s="94" t="s">
         <v>139</v>
       </c>
-      <c r="D140" s="114"/>
-      <c r="E140" s="114"/>
-      <c r="F140" s="114"/>
-      <c r="G140" s="114"/>
-      <c r="H140" s="114"/>
-      <c r="I140" s="114"/>
+      <c r="D140" s="94"/>
+      <c r="E140" s="94"/>
+      <c r="F140" s="94"/>
+      <c r="G140" s="94"/>
+      <c r="H140" s="94"/>
+      <c r="I140" s="94"/>
     </row>
     <row r="141" spans="1:9" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B141" s="97" t="s">
+      <c r="B141" s="93" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3819,13 +3848,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:I3"/>
-    <mergeCell ref="A12:I13"/>
-    <mergeCell ref="A24:I25"/>
-    <mergeCell ref="A86:I87"/>
-    <mergeCell ref="A99:I100"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="A33:A42"/>
     <mergeCell ref="A111:E111"/>
     <mergeCell ref="A123:E123"/>
     <mergeCell ref="A43:A53"/>
@@ -3834,6 +3856,13 @@
     <mergeCell ref="A61:A66"/>
     <mergeCell ref="A54:A60"/>
     <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A2:I3"/>
+    <mergeCell ref="A12:I13"/>
+    <mergeCell ref="A24:I25"/>
+    <mergeCell ref="A86:I87"/>
+    <mergeCell ref="A99:I100"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="A33:A42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ok lấy danh sách sản phẩm theo danh mục
</commit_message>
<xml_diff>
--- a/Database ToCoShopvs.xlsx
+++ b/Database ToCoShopvs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="155">
   <si>
     <t>No.</t>
   </si>
@@ -470,13 +470,16 @@
     <t>Lấy toàn bộ sản phẩm có thêm stockTotal mô tả số lượng sản phẩm tồn kho và totalPrice- giá sản phẩm theo mỗi [size và màu sắc] trong một danh mục nổi bật- theo id sản phẩm( hàng mới cập nhật) || StockTotal&gt;0</t>
   </si>
   <si>
-    <t>Lấy toàn bộ sản phẩm có thêm stockTotal mô tả số lượng sản phẩm tồn kho và totalPrice- giá sản phẩm theo mỗi [size và màu sắc] trong một danh mục( truyền params categoryId) || StockTotal&gt;0</t>
-  </si>
-  <si>
     <t>Lấy toàn bộ sản phẩm có thêm stockTotal mô tả số lượng sản phẩm tồn kho và totalPrice- giá sản phẩm theo mỗi [size và màu sắc] thuộc về một nhà phân phối( dựa theo params supplierId) || StockTotal&gt;0</t>
   </si>
   <si>
     <t>Lấy toàn bộ sản phẩm có thêm stockTotal mô tả số lượng sản phẩm tồn kho và totalPrice- giá sản phẩm theo mỗi [size và màu sắc] có trường mảng Array- promotionPosition- chứa cụm từ "Giảm sốc trong ngày" hoặc "Gợi ý trong tuần" || StockTotal&gt;0</t>
+  </si>
+  <si>
+    <t>Hien thi mac dinh là gia san pham thap nhat</t>
+  </si>
+  <si>
+    <t>Lấy toàn bộ sản phẩm có thêm stockTotal mô tả số lượng sản phẩm tồn kho và totalPrice- giá sản phẩm theo mỗi [size và màu sắc] trong một danh mục( truyền params categoryId) || StockTotal&gt;0 || Hien thi mac dinh gia thanh tien nho nhat.</t>
   </si>
 </sst>
 </file>
@@ -1091,45 +1094,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1150,14 +1119,48 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1485,28 +1488,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
     </row>
     <row r="3" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="110"/>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
+      <c r="A3" s="121"/>
+      <c r="B3" s="121"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
     </row>
     <row r="4" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
@@ -1647,28 +1650,28 @@
       <c r="I9" s="18"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="111" t="s">
+      <c r="A12" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="111"/>
-      <c r="C12" s="111"/>
-      <c r="D12" s="111"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
+      <c r="B12" s="122"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="122"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="112"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="112"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="112"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="123"/>
+      <c r="C13" s="123"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="123"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="39" t="s">
@@ -1847,28 +1850,28 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="113" t="s">
+      <c r="A24" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="113"/>
-      <c r="C24" s="113"/>
-      <c r="D24" s="113"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="113"/>
-      <c r="G24" s="113"/>
-      <c r="H24" s="113"/>
-      <c r="I24" s="113"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="124"/>
+      <c r="D24" s="124"/>
+      <c r="E24" s="124"/>
+      <c r="F24" s="124"/>
+      <c r="G24" s="124"/>
+      <c r="H24" s="124"/>
+      <c r="I24" s="124"/>
     </row>
     <row r="25" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="113"/>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="113"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="113"/>
-      <c r="G25" s="113"/>
-      <c r="H25" s="113"/>
-      <c r="I25" s="113"/>
+      <c r="A25" s="124"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="124"/>
+      <c r="D25" s="124"/>
+      <c r="E25" s="124"/>
+      <c r="F25" s="124"/>
+      <c r="G25" s="124"/>
+      <c r="H25" s="124"/>
+      <c r="I25" s="124"/>
     </row>
     <row r="26" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -2031,7 +2034,7 @@
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="117">
+      <c r="A33" s="128">
         <v>7</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -2048,7 +2051,7 @@
       <c r="I33" s="8"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="118"/>
+      <c r="A34" s="129"/>
       <c r="B34" s="4" t="s">
         <v>26</v>
       </c>
@@ -2067,7 +2070,7 @@
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="118"/>
+      <c r="A35" s="129"/>
       <c r="B35" s="4" t="s">
         <v>25</v>
       </c>
@@ -2088,7 +2091,7 @@
       <c r="I35" s="4"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="118"/>
+      <c r="A36" s="129"/>
       <c r="B36" s="4" t="s">
         <v>54</v>
       </c>
@@ -2107,7 +2110,7 @@
       <c r="I36" s="4"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="118"/>
+      <c r="A37" s="129"/>
       <c r="B37" s="4" t="s">
         <v>53</v>
       </c>
@@ -2126,7 +2129,7 @@
       <c r="I37" s="4"/>
     </row>
     <row r="38" spans="1:9" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A38" s="118"/>
+      <c r="A38" s="129"/>
       <c r="B38" s="23" t="s">
         <v>27</v>
       </c>
@@ -2143,7 +2146,7 @@
       <c r="I38" s="91"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="118"/>
+      <c r="A39" s="129"/>
       <c r="B39" s="26" t="s">
         <v>51</v>
       </c>
@@ -2162,7 +2165,7 @@
       <c r="I39" s="4"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="118"/>
+      <c r="A40" s="129"/>
       <c r="B40" s="26" t="s">
         <v>109</v>
       </c>
@@ -2181,7 +2184,7 @@
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="118"/>
+      <c r="A41" s="129"/>
       <c r="B41" s="26" t="s">
         <v>110</v>
       </c>
@@ -2200,7 +2203,7 @@
       <c r="I41" s="4"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="119"/>
+      <c r="A42" s="130"/>
       <c r="B42" s="26" t="s">
         <v>52</v>
       </c>
@@ -2219,7 +2222,7 @@
       <c r="I42" s="4"/>
     </row>
     <row r="43" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="117">
+      <c r="A43" s="128">
         <v>8</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -2238,7 +2241,7 @@
       <c r="I43" s="8"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="118"/>
+      <c r="A44" s="129"/>
       <c r="B44" s="4" t="s">
         <v>96</v>
       </c>
@@ -2257,7 +2260,7 @@
       <c r="I44" s="4"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="118"/>
+      <c r="A45" s="129"/>
       <c r="B45" s="4" t="s">
         <v>54</v>
       </c>
@@ -2276,7 +2279,7 @@
       <c r="I45" s="4"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="118"/>
+      <c r="A46" s="129"/>
       <c r="B46" s="4" t="s">
         <v>53</v>
       </c>
@@ -2295,7 +2298,7 @@
       <c r="I46" s="4"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="118"/>
+      <c r="A47" s="129"/>
       <c r="B47" s="4" t="s">
         <v>26</v>
       </c>
@@ -2314,7 +2317,7 @@
       <c r="I47" s="4"/>
     </row>
     <row r="48" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A48" s="118"/>
+      <c r="A48" s="129"/>
       <c r="B48" s="23" t="s">
         <v>27</v>
       </c>
@@ -2325,15 +2328,15 @@
       <c r="E48" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="F48" s="115" t="s">
+      <c r="F48" s="126" t="s">
         <v>74</v>
       </c>
-      <c r="G48" s="115"/>
-      <c r="H48" s="115"/>
-      <c r="I48" s="116"/>
+      <c r="G48" s="126"/>
+      <c r="H48" s="126"/>
+      <c r="I48" s="127"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="118"/>
+      <c r="A49" s="129"/>
       <c r="B49" s="26" t="s">
         <v>51</v>
       </c>
@@ -2352,7 +2355,7 @@
       <c r="I49" s="4"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="118"/>
+      <c r="A50" s="129"/>
       <c r="B50" s="26" t="s">
         <v>109</v>
       </c>
@@ -2371,7 +2374,7 @@
       <c r="I50" s="4"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="118"/>
+      <c r="A51" s="129"/>
       <c r="B51" s="26" t="s">
         <v>110</v>
       </c>
@@ -2390,7 +2393,7 @@
       <c r="I51" s="4"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="118"/>
+      <c r="A52" s="129"/>
       <c r="B52" s="26" t="s">
         <v>52</v>
       </c>
@@ -2409,7 +2412,7 @@
       <c r="I52" s="4"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="119"/>
+      <c r="A53" s="130"/>
       <c r="B53" s="4" t="s">
         <v>49</v>
       </c>
@@ -2428,7 +2431,7 @@
       <c r="I53" s="4"/>
     </row>
     <row r="54" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="117">
+      <c r="A54" s="128">
         <v>9</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -2447,7 +2450,7 @@
       <c r="I54" s="8"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="118"/>
+      <c r="A55" s="129"/>
       <c r="B55" s="4" t="s">
         <v>55</v>
       </c>
@@ -2464,7 +2467,7 @@
       <c r="I55" s="4"/>
     </row>
     <row r="56" spans="1:9" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A56" s="118"/>
+      <c r="A56" s="129"/>
       <c r="B56" s="23" t="s">
         <v>57</v>
       </c>
@@ -2472,16 +2475,16 @@
         <v>38</v>
       </c>
       <c r="D56" s="25"/>
-      <c r="E56" s="120" t="s">
+      <c r="E56" s="131" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="115"/>
-      <c r="G56" s="115"/>
-      <c r="H56" s="115"/>
-      <c r="I56" s="116"/>
+      <c r="F56" s="126"/>
+      <c r="G56" s="126"/>
+      <c r="H56" s="126"/>
+      <c r="I56" s="127"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="118"/>
+      <c r="A57" s="129"/>
       <c r="B57" s="26" t="s">
         <v>58</v>
       </c>
@@ -2498,7 +2501,7 @@
       <c r="I57" s="4"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="118"/>
+      <c r="A58" s="129"/>
       <c r="B58" s="26" t="s">
         <v>91</v>
       </c>
@@ -2515,7 +2518,7 @@
       <c r="I58" s="4"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="118"/>
+      <c r="A59" s="129"/>
       <c r="B59" s="26" t="s">
         <v>59</v>
       </c>
@@ -2534,7 +2537,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="119"/>
+      <c r="A60" s="130"/>
       <c r="B60" s="26" t="s">
         <v>60</v>
       </c>
@@ -2553,7 +2556,7 @@
       <c r="I60" s="4"/>
     </row>
     <row r="61" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="121">
+      <c r="A61" s="132">
         <v>10</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -2570,7 +2573,7 @@
       <c r="I61" s="8"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="121"/>
+      <c r="A62" s="132"/>
       <c r="B62" s="4" t="s">
         <v>112</v>
       </c>
@@ -2589,7 +2592,7 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="121"/>
+      <c r="A63" s="132"/>
       <c r="B63" s="4" t="s">
         <v>117</v>
       </c>
@@ -2604,7 +2607,7 @@
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="121"/>
+      <c r="A64" s="132"/>
       <c r="B64" s="4" t="s">
         <v>41</v>
       </c>
@@ -2619,7 +2622,7 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="121"/>
+      <c r="A65" s="132"/>
       <c r="B65" s="4" t="s">
         <v>43</v>
       </c>
@@ -2634,7 +2637,7 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="121"/>
+      <c r="A66" s="132"/>
       <c r="B66" s="4" t="s">
         <v>44</v>
       </c>
@@ -2649,7 +2652,7 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="117">
+      <c r="A67" s="128">
         <v>11</v>
       </c>
       <c r="B67" s="8" t="s">
@@ -2666,7 +2669,7 @@
       <c r="I67" s="8"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="118"/>
+      <c r="A68" s="129"/>
       <c r="B68" s="4" t="s">
         <v>101</v>
       </c>
@@ -2685,7 +2688,7 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="118"/>
+      <c r="A69" s="129"/>
       <c r="B69" s="4" t="s">
         <v>102</v>
       </c>
@@ -2704,7 +2707,7 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="119"/>
+      <c r="A70" s="130"/>
       <c r="B70" s="4" t="s">
         <v>93</v>
       </c>
@@ -2721,28 +2724,28 @@
       <c r="I70" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="111" t="s">
+      <c r="A73" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="B73" s="111"/>
-      <c r="C73" s="111"/>
-      <c r="D73" s="111"/>
-      <c r="E73" s="111"/>
-      <c r="F73" s="111"/>
-      <c r="G73" s="111"/>
-      <c r="H73" s="111"/>
-      <c r="I73" s="111"/>
+      <c r="B73" s="122"/>
+      <c r="C73" s="122"/>
+      <c r="D73" s="122"/>
+      <c r="E73" s="122"/>
+      <c r="F73" s="122"/>
+      <c r="G73" s="122"/>
+      <c r="H73" s="122"/>
+      <c r="I73" s="122"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="112"/>
-      <c r="B74" s="112"/>
-      <c r="C74" s="112"/>
-      <c r="D74" s="112"/>
-      <c r="E74" s="112"/>
-      <c r="F74" s="112"/>
-      <c r="G74" s="112"/>
-      <c r="H74" s="112"/>
-      <c r="I74" s="112"/>
+      <c r="A74" s="123"/>
+      <c r="B74" s="123"/>
+      <c r="C74" s="123"/>
+      <c r="D74" s="123"/>
+      <c r="E74" s="123"/>
+      <c r="F74" s="123"/>
+      <c r="G74" s="123"/>
+      <c r="H74" s="123"/>
+      <c r="I74" s="123"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="39" t="s">
@@ -2917,28 +2920,28 @@
       <c r="I82" s="44"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="109" t="s">
+      <c r="A86" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="B86" s="109"/>
-      <c r="C86" s="109"/>
-      <c r="D86" s="109"/>
-      <c r="E86" s="109"/>
-      <c r="F86" s="109"/>
-      <c r="G86" s="109"/>
-      <c r="H86" s="109"/>
-      <c r="I86" s="109"/>
+      <c r="B86" s="120"/>
+      <c r="C86" s="120"/>
+      <c r="D86" s="120"/>
+      <c r="E86" s="120"/>
+      <c r="F86" s="120"/>
+      <c r="G86" s="120"/>
+      <c r="H86" s="120"/>
+      <c r="I86" s="120"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="114"/>
-      <c r="B87" s="114"/>
-      <c r="C87" s="114"/>
-      <c r="D87" s="114"/>
-      <c r="E87" s="114"/>
-      <c r="F87" s="114"/>
-      <c r="G87" s="114"/>
-      <c r="H87" s="114"/>
-      <c r="I87" s="114"/>
+      <c r="A87" s="125"/>
+      <c r="B87" s="125"/>
+      <c r="C87" s="125"/>
+      <c r="D87" s="125"/>
+      <c r="E87" s="125"/>
+      <c r="F87" s="125"/>
+      <c r="G87" s="125"/>
+      <c r="H87" s="125"/>
+      <c r="I87" s="125"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="33" t="s">
@@ -3082,28 +3085,28 @@
       <c r="A95" s="61"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="109" t="s">
+      <c r="A99" s="120" t="s">
         <v>75</v>
       </c>
-      <c r="B99" s="109"/>
-      <c r="C99" s="109"/>
-      <c r="D99" s="109"/>
-      <c r="E99" s="109"/>
-      <c r="F99" s="109"/>
-      <c r="G99" s="109"/>
-      <c r="H99" s="109"/>
-      <c r="I99" s="109"/>
+      <c r="B99" s="120"/>
+      <c r="C99" s="120"/>
+      <c r="D99" s="120"/>
+      <c r="E99" s="120"/>
+      <c r="F99" s="120"/>
+      <c r="G99" s="120"/>
+      <c r="H99" s="120"/>
+      <c r="I99" s="120"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="114"/>
-      <c r="B100" s="114"/>
-      <c r="C100" s="114"/>
-      <c r="D100" s="114"/>
-      <c r="E100" s="114"/>
-      <c r="F100" s="114"/>
-      <c r="G100" s="114"/>
-      <c r="H100" s="114"/>
-      <c r="I100" s="114"/>
+      <c r="A100" s="125"/>
+      <c r="B100" s="125"/>
+      <c r="C100" s="125"/>
+      <c r="D100" s="125"/>
+      <c r="E100" s="125"/>
+      <c r="F100" s="125"/>
+      <c r="G100" s="125"/>
+      <c r="H100" s="125"/>
+      <c r="I100" s="125"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="33" t="s">
@@ -3261,13 +3264,13 @@
       <c r="I107" s="68"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="126" t="s">
+      <c r="A111" s="116" t="s">
         <v>79</v>
       </c>
-      <c r="B111" s="127"/>
-      <c r="C111" s="127"/>
-      <c r="D111" s="127"/>
-      <c r="E111" s="127"/>
+      <c r="B111" s="117"/>
+      <c r="C111" s="117"/>
+      <c r="D111" s="117"/>
+      <c r="E111" s="117"/>
       <c r="F111" s="71"/>
       <c r="G111" s="71"/>
       <c r="H111" s="71"/>
@@ -3505,13 +3508,13 @@
       <c r="I122" s="85"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="128" t="s">
+      <c r="A123" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="B123" s="129"/>
-      <c r="C123" s="129"/>
-      <c r="D123" s="129"/>
-      <c r="E123" s="129"/>
+      <c r="B123" s="119"/>
+      <c r="C123" s="119"/>
+      <c r="D123" s="119"/>
+      <c r="E123" s="119"/>
       <c r="F123" s="93"/>
       <c r="G123" s="93"/>
       <c r="H123" s="93"/>
@@ -3711,7 +3714,7 @@
       <c r="I132" s="30"/>
     </row>
     <row r="133" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="122">
+      <c r="A133" s="112">
         <v>9</v>
       </c>
       <c r="B133" s="96" t="s">
@@ -3732,7 +3735,7 @@
       </c>
     </row>
     <row r="134" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="123"/>
+      <c r="A134" s="113"/>
       <c r="B134" s="18" t="s">
         <v>132</v>
       </c>
@@ -3752,7 +3755,7 @@
       <c r="L134" s="100"/>
     </row>
     <row r="135" spans="1:12" s="92" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="124"/>
+      <c r="A135" s="114"/>
       <c r="B135" s="18" t="s">
         <v>133</v>
       </c>
@@ -3774,7 +3777,7 @@
       <c r="L135" s="100"/>
     </row>
     <row r="136" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="125">
+      <c r="A136" s="115">
         <v>10</v>
       </c>
       <c r="B136" s="62" t="s">
@@ -3791,7 +3794,7 @@
       <c r="I136" s="62"/>
     </row>
     <row r="137" spans="1:12" s="104" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A137" s="125"/>
+      <c r="A137" s="115"/>
       <c r="B137" s="101" t="s">
         <v>9</v>
       </c>
@@ -3810,7 +3813,7 @@
       <c r="I137" s="101"/>
     </row>
     <row r="138" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="125"/>
+      <c r="A138" s="115"/>
       <c r="B138" s="18" t="s">
         <v>135</v>
       </c>
@@ -3827,7 +3830,7 @@
       <c r="I138" s="62"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A139" s="125"/>
+      <c r="A139" s="115"/>
       <c r="B139" s="18" t="s">
         <v>117</v>
       </c>
@@ -3844,7 +3847,7 @@
       <c r="I139" s="18"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A140" s="125"/>
+      <c r="A140" s="115"/>
       <c r="B140" s="18" t="s">
         <v>83</v>
       </c>
@@ -3859,7 +3862,7 @@
       <c r="I140" s="18"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A141" s="125"/>
+      <c r="A141" s="115"/>
       <c r="B141" s="18" t="s">
         <v>43</v>
       </c>
@@ -3874,7 +3877,7 @@
       <c r="I141" s="18"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A142" s="125"/>
+      <c r="A142" s="115"/>
       <c r="B142" s="18" t="s">
         <v>44</v>
       </c>
@@ -3933,6 +3936,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A67:A70"/>
     <mergeCell ref="A133:A135"/>
     <mergeCell ref="A136:A142"/>
     <mergeCell ref="A111:E111"/>
@@ -3949,7 +3953,6 @@
     <mergeCell ref="E56:I56"/>
     <mergeCell ref="A61:A66"/>
     <mergeCell ref="A54:A60"/>
-    <mergeCell ref="A67:A70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3958,10 +3961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:D16"/>
+  <dimension ref="A4:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3974,6 +3977,11 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="108" t="s">
+        <v>153</v>
+      </c>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>140</v>
@@ -3995,7 +4003,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="107" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
         <v>141</v>
@@ -4006,14 +4014,14 @@
         <v>3</v>
       </c>
       <c r="B9" s="107" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="130">
+      <c r="A10" s="133">
         <v>4</v>
       </c>
       <c r="B10" s="108" t="s">
@@ -4024,7 +4032,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="130"/>
+      <c r="A11" s="133"/>
       <c r="B11" s="107" t="s">
         <v>147</v>
       </c>
@@ -4033,7 +4041,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="130"/>
+      <c r="A12" s="133"/>
       <c r="B12" s="107" t="s">
         <v>148</v>
       </c>
@@ -4068,7 +4076,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
         <v>141</v>
@@ -4077,14 +4085,14 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="133" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="131">
+    <row r="16" spans="1:4" s="111" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="109">
         <v>8</v>
       </c>
-      <c r="B16" s="132" t="s">
+      <c r="B16" s="110" t="s">
         <v>145</v>
       </c>
-      <c r="D16" s="133" t="s">
+      <c r="D16" s="111" t="s">
         <v>146</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update finish create an order
</commit_message>
<xml_diff>
--- a/Database ToCoShopvs.xlsx
+++ b/Database ToCoShopvs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10512"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10512" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="152">
   <si>
     <t>No.</t>
   </si>
@@ -468,6 +468,9 @@
   </si>
   <si>
     <t>UNIQUE -Reference to collection Login</t>
+  </si>
+  <si>
+    <t>Liệt kê danh sách sản phẩm thêm trường bestDiscount chứa discount của mẫu attribute giảm giá lớn nhất- đây là danh sách sản phẩm còn hàng trong kho</t>
   </si>
 </sst>
 </file>
@@ -660,28 +663,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -693,10 +691,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -1004,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1047,54 +1050,54 @@
       <c r="I3" s="19"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
+      <c r="A5" s="16">
         <v>1</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18" t="s">
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="18"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
@@ -1150,7 +1153,7 @@
       <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1186,54 +1189,54 @@
       <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18">
+      <c r="A14" s="16">
         <v>1</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18" t="s">
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18" t="s">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
@@ -1334,7 +1337,7 @@
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -1370,54 +1373,54 @@
       <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18">
+      <c r="A25" s="16">
         <v>1</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18" t="s">
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18" t="s">
+      <c r="G25" s="16"/>
+      <c r="H25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="16"/>
     </row>
     <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
@@ -1530,13 +1533,13 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="23">
+      <c r="A31" s="21">
         <v>7</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D31" s="5"/>
@@ -1547,7 +1550,7 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
+      <c r="A32" s="21"/>
       <c r="B32" s="5" t="s">
         <v>25</v>
       </c>
@@ -1566,7 +1569,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
+      <c r="A33" s="21"/>
       <c r="B33" s="5" t="s">
         <v>24</v>
       </c>
@@ -1587,7 +1590,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
+      <c r="A34" s="21"/>
       <c r="B34" s="5" t="s">
         <v>52</v>
       </c>
@@ -1606,7 +1609,7 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="A35" s="21"/>
       <c r="B35" s="5" t="s">
         <v>51</v>
       </c>
@@ -1625,26 +1628,26 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A36" s="23"/>
-      <c r="B36" s="24" t="s">
+      <c r="A36" s="21"/>
+      <c r="B36" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="18" t="s">
         <v>59</v>
       </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="25" t="s">
+      <c r="F36" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="27"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="5" t="s">
         <v>49</v>
       </c>
@@ -1663,7 +1666,7 @@
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="5" t="s">
         <v>99</v>
       </c>
@@ -1682,7 +1685,7 @@
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="5" t="s">
         <v>100</v>
       </c>
@@ -1701,7 +1704,7 @@
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
+      <c r="A40" s="21"/>
       <c r="B40" s="5" t="s">
         <v>50</v>
       </c>
@@ -1720,17 +1723,17 @@
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28">
+      <c r="A41" s="22">
         <v>8</v>
       </c>
-      <c r="B41" s="18" t="s">
+      <c r="B41" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D41" s="5"/>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="5"/>
@@ -1739,7 +1742,7 @@
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="5" t="s">
         <v>90</v>
       </c>
@@ -1748,7 +1751,7 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G42" s="5"/>
@@ -1758,7 +1761,7 @@
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5" t="s">
         <v>52</v>
       </c>
@@ -1777,7 +1780,7 @@
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="5" t="s">
         <v>51</v>
       </c>
@@ -1796,7 +1799,7 @@
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="5" t="s">
         <v>25</v>
       </c>
@@ -1815,26 +1818,26 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A46" s="28"/>
-      <c r="B46" s="24" t="s">
+      <c r="A46" s="22"/>
+      <c r="B46" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C46" s="18" t="s">
         <v>59</v>
       </c>
       <c r="D46" s="5"/>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="5" t="s">
         <v>49</v>
       </c>
@@ -1853,7 +1856,7 @@
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>99</v>
       </c>
@@ -1872,7 +1875,7 @@
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
+      <c r="A49" s="22"/>
       <c r="B49" s="5" t="s">
         <v>100</v>
       </c>
@@ -1891,7 +1894,7 @@
       <c r="I49" s="5"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
+      <c r="A50" s="22"/>
       <c r="B50" s="5" t="s">
         <v>50</v>
       </c>
@@ -1910,7 +1913,7 @@
       <c r="I50" s="5"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
+      <c r="A51" s="22"/>
       <c r="B51" s="5" t="s">
         <v>47</v>
       </c>
@@ -1929,17 +1932,17 @@
       <c r="I51" s="5"/>
     </row>
     <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="23">
+      <c r="A52" s="21">
         <v>9</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18" t="s">
+      <c r="D52" s="16"/>
+      <c r="E52" s="16" t="s">
         <v>17</v>
       </c>
       <c r="F52" s="5"/>
@@ -1948,7 +1951,7 @@
       <c r="I52" s="5"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="23"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="5" t="s">
         <v>53</v>
       </c>
@@ -1965,24 +1968,24 @@
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="1:9" s="2" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24" t="s">
+      <c r="A54" s="21"/>
+      <c r="B54" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="24" t="s">
+      <c r="C54" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="24"/>
-      <c r="E54" s="29" t="s">
+      <c r="D54" s="18"/>
+      <c r="E54" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="29"/>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
+      <c r="A55" s="21"/>
       <c r="B55" s="5" t="s">
         <v>56</v>
       </c>
@@ -1999,7 +2002,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="23"/>
+      <c r="A56" s="21"/>
       <c r="B56" s="5" t="s">
         <v>87</v>
       </c>
@@ -2016,7 +2019,7 @@
       <c r="I56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="23"/>
+      <c r="A57" s="21"/>
       <c r="B57" s="5" t="s">
         <v>57</v>
       </c>
@@ -2033,7 +2036,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="23"/>
+      <c r="A58" s="21"/>
       <c r="B58" s="5" t="s">
         <v>58</v>
       </c>
@@ -2052,13 +2055,13 @@
       </c>
     </row>
     <row r="59" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="23">
+      <c r="A59" s="21">
         <v>10</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B59" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C59" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D59" s="5"/>
@@ -2069,7 +2072,7 @@
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="23"/>
+      <c r="A60" s="21"/>
       <c r="B60" s="5" t="s">
         <v>145</v>
       </c>
@@ -2078,7 +2081,7 @@
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
-      <c r="F60" s="18" t="s">
+      <c r="F60" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G60" s="5"/>
@@ -2088,7 +2091,7 @@
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="23"/>
+      <c r="A61" s="21"/>
       <c r="B61" s="5" t="s">
         <v>39</v>
       </c>
@@ -2103,7 +2106,7 @@
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="23"/>
+      <c r="A62" s="21"/>
       <c r="B62" s="5" t="s">
         <v>41</v>
       </c>
@@ -2118,7 +2121,7 @@
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="23"/>
+      <c r="A63" s="21"/>
       <c r="B63" s="5" t="s">
         <v>42</v>
       </c>
@@ -2133,13 +2136,13 @@
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="23">
+      <c r="A64" s="21">
         <v>11</v>
       </c>
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="18" t="s">
+      <c r="C64" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D64" s="5"/>
@@ -2150,7 +2153,7 @@
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="23"/>
+      <c r="A65" s="21"/>
       <c r="B65" s="5" t="s">
         <v>92</v>
       </c>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
-      <c r="F65" s="18" t="s">
+      <c r="F65" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G65" s="5"/>
@@ -2169,7 +2172,7 @@
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="23"/>
+      <c r="A66" s="21"/>
       <c r="B66" s="5" t="s">
         <v>93</v>
       </c>
@@ -2188,7 +2191,7 @@
       <c r="I66" s="5"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="23"/>
+      <c r="A67" s="21"/>
       <c r="B67" s="5" t="s">
         <v>88</v>
       </c>
@@ -2229,54 +2232,54 @@
       <c r="I71" s="19"/>
     </row>
     <row r="72" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="18" t="s">
+      <c r="A72" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B72" s="18" t="s">
+      <c r="B72" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="18" t="s">
+      <c r="C72" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D72" s="18" t="s">
+      <c r="D72" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="18" t="s">
+      <c r="E72" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="18" t="s">
+      <c r="F72" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G72" s="18" t="s">
+      <c r="G72" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H72" s="18" t="s">
+      <c r="H72" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I72" s="18" t="s">
+      <c r="I72" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="18">
+      <c r="A73" s="16">
         <v>1</v>
       </c>
-      <c r="B73" s="18" t="s">
+      <c r="B73" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="18" t="s">
+      <c r="C73" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="18" t="s">
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G73" s="18"/>
-      <c r="H73" s="18" t="s">
+      <c r="G73" s="16"/>
+      <c r="H73" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I73" s="18"/>
+      <c r="I73" s="16"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
@@ -2427,54 +2430,54 @@
       <c r="I84" s="19"/>
     </row>
     <row r="85" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="18" t="s">
+      <c r="A85" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C85" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="18" t="s">
+      <c r="D85" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="18" t="s">
+      <c r="E85" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F85" s="18" t="s">
+      <c r="F85" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G85" s="18" t="s">
+      <c r="G85" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H85" s="18" t="s">
+      <c r="H85" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I85" s="18" t="s">
+      <c r="I85" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="18">
+      <c r="A86" s="16">
         <v>1</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="C86" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D86" s="18"/>
-      <c r="E86" s="18"/>
-      <c r="F86" s="18" t="s">
+      <c r="D86" s="16"/>
+      <c r="E86" s="16"/>
+      <c r="F86" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G86" s="18"/>
-      <c r="H86" s="18" t="s">
+      <c r="G86" s="16"/>
+      <c r="H86" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I86" s="18"/>
+      <c r="I86" s="16"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
@@ -2596,54 +2599,54 @@
       <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="18" t="s">
+      <c r="A98" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B98" s="18" t="s">
+      <c r="B98" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C98" s="18" t="s">
+      <c r="C98" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D98" s="18" t="s">
+      <c r="D98" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E98" s="18" t="s">
+      <c r="E98" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F98" s="18" t="s">
+      <c r="F98" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G98" s="18" t="s">
+      <c r="G98" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H98" s="18" t="s">
+      <c r="H98" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I98" s="18" t="s">
+      <c r="I98" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="18">
+      <c r="A99" s="16">
         <v>1</v>
       </c>
-      <c r="B99" s="18" t="s">
+      <c r="B99" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C99" s="18" t="s">
+      <c r="C99" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D99" s="18"/>
-      <c r="E99" s="18"/>
-      <c r="F99" s="18" t="s">
+      <c r="D99" s="16"/>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G99" s="18"/>
-      <c r="H99" s="18" t="s">
+      <c r="G99" s="16"/>
+      <c r="H99" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I99" s="18"/>
+      <c r="I99" s="16"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
@@ -2775,54 +2778,54 @@
       <c r="I108" s="19"/>
     </row>
     <row r="109" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="18" t="s">
+      <c r="A109" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B109" s="18" t="s">
+      <c r="B109" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C109" s="18" t="s">
+      <c r="C109" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D109" s="18" t="s">
+      <c r="D109" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E109" s="18" t="s">
+      <c r="E109" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F109" s="18" t="s">
+      <c r="F109" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G109" s="18" t="s">
+      <c r="G109" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H109" s="18" t="s">
+      <c r="H109" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I109" s="18" t="s">
+      <c r="I109" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="18">
+      <c r="A110" s="16">
         <v>1</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C110" s="18" t="s">
+      <c r="C110" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D110" s="18">
+      <c r="D110" s="16">
         <v>50</v>
       </c>
-      <c r="E110" s="18"/>
-      <c r="F110" s="18" t="s">
+      <c r="E110" s="16"/>
+      <c r="F110" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G110" s="18"/>
-      <c r="H110" s="18"/>
-      <c r="I110" s="18"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="16"/>
+      <c r="I110" s="16"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="5">
@@ -2991,89 +2994,89 @@
       <c r="I118" s="5"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="16"/>
-      <c r="B119" s="16"/>
-      <c r="C119" s="16"/>
-      <c r="D119" s="16"/>
-      <c r="E119" s="16"/>
-      <c r="F119" s="16"/>
-      <c r="G119" s="16"/>
-      <c r="H119" s="16"/>
-      <c r="I119" s="16"/>
+      <c r="A119" s="15"/>
+      <c r="B119" s="15"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+      <c r="I119" s="15"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="21" t="s">
+      <c r="A120" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="B120" s="21"/>
-      <c r="C120" s="21"/>
-      <c r="D120" s="21"/>
-      <c r="E120" s="21"/>
-      <c r="F120" s="21"/>
-      <c r="G120" s="21"/>
-      <c r="H120" s="21"/>
-      <c r="I120" s="21"/>
+      <c r="B120" s="27"/>
+      <c r="C120" s="27"/>
+      <c r="D120" s="27"/>
+      <c r="E120" s="27"/>
+      <c r="F120" s="27"/>
+      <c r="G120" s="27"/>
+      <c r="H120" s="27"/>
+      <c r="I120" s="27"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="22"/>
-      <c r="B121" s="22"/>
-      <c r="C121" s="22"/>
-      <c r="D121" s="22"/>
-      <c r="E121" s="22"/>
-      <c r="F121" s="22"/>
-      <c r="G121" s="22"/>
-      <c r="H121" s="22"/>
-      <c r="I121" s="22"/>
+      <c r="A121" s="28"/>
+      <c r="B121" s="28"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="28"/>
+      <c r="F121" s="28"/>
+      <c r="G121" s="28"/>
+      <c r="H121" s="28"/>
+      <c r="I121" s="28"/>
     </row>
     <row r="122" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="18" t="s">
+      <c r="A122" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C122" s="18" t="s">
+      <c r="C122" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D122" s="18" t="s">
+      <c r="D122" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E122" s="18" t="s">
+      <c r="E122" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F122" s="18" t="s">
+      <c r="F122" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G122" s="18" t="s">
+      <c r="G122" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H122" s="18" t="s">
+      <c r="H122" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I122" s="18" t="s">
+      <c r="I122" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="18">
+      <c r="A123" s="16">
         <v>1</v>
       </c>
-      <c r="B123" s="18" t="s">
+      <c r="B123" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C123" s="18" t="s">
+      <c r="C123" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D123" s="18"/>
-      <c r="E123" s="18"/>
-      <c r="F123" s="18" t="s">
+      <c r="D123" s="16"/>
+      <c r="E123" s="16"/>
+      <c r="F123" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G123" s="18"/>
-      <c r="H123" s="18" t="s">
+      <c r="G123" s="16"/>
+      <c r="H123" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I123" s="18"/>
+      <c r="I123" s="16"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="5">
@@ -3127,7 +3130,7 @@
       </c>
       <c r="D126" s="5"/>
       <c r="E126" s="5"/>
-      <c r="F126" s="18" t="s">
+      <c r="F126" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G126" s="5"/>
@@ -3148,7 +3151,7 @@
       </c>
       <c r="D127" s="5"/>
       <c r="E127" s="5"/>
-      <c r="F127" s="18" t="s">
+      <c r="F127" s="16" t="s">
         <v>33</v>
       </c>
       <c r="G127" s="5"/>
@@ -3219,13 +3222,13 @@
       <c r="I130" s="5"/>
     </row>
     <row r="131" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="23">
+      <c r="A131" s="21">
         <v>9</v>
       </c>
-      <c r="B131" s="18" t="s">
+      <c r="B131" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C131" s="18" t="s">
+      <c r="C131" s="16" t="s">
         <v>86</v>
       </c>
       <c r="D131" s="5"/>
@@ -3238,7 +3241,7 @@
       <c r="I131" s="5"/>
     </row>
     <row r="132" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="23"/>
+      <c r="A132" s="21"/>
       <c r="B132" s="5" t="s">
         <v>119</v>
       </c>
@@ -3253,7 +3256,7 @@
       <c r="L132" s="7"/>
     </row>
     <row r="133" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="23"/>
+      <c r="A133" s="21"/>
       <c r="B133" s="5" t="s">
         <v>120</v>
       </c>
@@ -3271,13 +3274,13 @@
       <c r="L133" s="7"/>
     </row>
     <row r="134" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="23">
+      <c r="A134" s="21">
         <v>10</v>
       </c>
-      <c r="B134" s="18" t="s">
+      <c r="B134" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C134" s="18" t="s">
+      <c r="C134" s="16" t="s">
         <v>86</v>
       </c>
       <c r="D134" s="5"/>
@@ -3288,7 +3291,7 @@
       <c r="I134" s="5"/>
     </row>
     <row r="135" spans="1:12" s="8" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A135" s="23"/>
+      <c r="A135" s="21"/>
       <c r="B135" s="5" t="s">
         <v>9</v>
       </c>
@@ -3307,7 +3310,7 @@
       <c r="I135" s="5"/>
     </row>
     <row r="136" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="23"/>
+      <c r="A136" s="21"/>
       <c r="B136" s="5" t="s">
         <v>122</v>
       </c>
@@ -3324,7 +3327,7 @@
       <c r="I136" s="5"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A137" s="23"/>
+      <c r="A137" s="21"/>
       <c r="B137" s="5" t="s">
         <v>105</v>
       </c>
@@ -3341,7 +3344,7 @@
       <c r="I137" s="5"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A138" s="23"/>
+      <c r="A138" s="21"/>
       <c r="B138" s="5" t="s">
         <v>80</v>
       </c>
@@ -3356,7 +3359,7 @@
       <c r="I138" s="5"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A139" s="23"/>
+      <c r="A139" s="21"/>
       <c r="B139" s="5" t="s">
         <v>41</v>
       </c>
@@ -3371,7 +3374,7 @@
       <c r="I139" s="5"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A140" s="23"/>
+      <c r="A140" s="21"/>
       <c r="B140" s="5" t="s">
         <v>42</v>
       </c>
@@ -3430,6 +3433,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A134:A140"/>
+    <mergeCell ref="A107:I108"/>
+    <mergeCell ref="A120:I121"/>
     <mergeCell ref="A2:I3"/>
     <mergeCell ref="A11:I12"/>
     <mergeCell ref="A22:I23"/>
@@ -3444,10 +3451,6 @@
     <mergeCell ref="A52:A58"/>
     <mergeCell ref="F36:I36"/>
     <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A134:A140"/>
-    <mergeCell ref="A107:I108"/>
-    <mergeCell ref="A120:I121"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3456,10 +3459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:D16"/>
+  <dimension ref="A4:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3516,7 +3519,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
+      <c r="A10" s="29">
         <v>4</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -3527,7 +3530,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="10" t="s">
         <v>134</v>
       </c>
@@ -3536,7 +3539,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="10" t="s">
         <v>135</v>
       </c>
@@ -3589,6 +3592,14 @@
       </c>
       <c r="D16" s="14" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>